<commit_message>
sorting and table header is fix
</commit_message>
<xml_diff>
--- a/lenovo.xlsx
+++ b/lenovo.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Tutorials" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tutorials!$A$1:$K$67</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="34">
   <si>
     <t>Id</t>
   </si>
@@ -49,7 +52,7 @@
     <t>accessoriesGuarante</t>
   </si>
   <si>
-    <t>Lenovo Smart Tab M10 FHD Plus</t>
+    <t>Varsha Lenovo Smart Tab M10 FHD Plus</t>
   </si>
   <si>
     <t>8gb</t>
@@ -64,19 +67,28 @@
     <t>Octa Core</t>
   </si>
   <si>
+    <t>2 year</t>
+  </si>
+  <si>
+    <t>1 Months</t>
+  </si>
+  <si>
+    <t>Redmi Note 9 Pro</t>
+  </si>
+  <si>
+    <t>20MP</t>
+  </si>
+  <si>
     <t>1 year</t>
   </si>
   <si>
     <t>6 Months</t>
   </si>
   <si>
-    <t>Redmi Note 9 Pro</t>
-  </si>
-  <si>
     <t>Redmi Note 7 Pro</t>
   </si>
   <si>
-    <t>Mi Mix 2</t>
+    <t>4GB</t>
   </si>
   <si>
     <t>Xiaomi 11i Hypercharge 5G</t>
@@ -91,13 +103,22 @@
     <t>Redmi Note 9.0 Pro</t>
   </si>
   <si>
-    <t>Redmi Note 7.5 Pro</t>
+    <t>Lenovo Smart Tab M10</t>
+  </si>
+  <si>
+    <t>Lenovo Smart Tab M10 FHD Plus</t>
   </si>
   <si>
     <t>Lenovo Smart Tab M10 FHD Plus octa</t>
   </si>
   <si>
-    <t>Lenovo Smart Tab M10</t>
+    <t>256gb</t>
+  </si>
+  <si>
+    <t>Mi Mix 2</t>
+  </si>
+  <si>
+    <t>Redmi Note 7.5 Pro</t>
   </si>
 </sst>
 </file>
@@ -105,10 +126,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -120,22 +141,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -143,6 +157,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,6 +193,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -194,19 +231,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,14 +263,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,30 +278,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,12 +297,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -297,7 +312,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,43 +462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -357,109 +474,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -476,23 +497,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,18 +520,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,28 +574,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,148 +596,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1048,8 +1069,8 @@
   <sheetPr/>
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1091,7 +1112,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1126,7 +1147,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1144,7 +1165,7 @@
         <v>256</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -1153,18 +1174,18 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1188,21 +1209,21 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1214,7 +1235,7 @@
         <v>256</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -1223,18 +1244,18 @@
         <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -1258,18 +1279,18 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -1284,7 +1305,7 @@
         <v>256</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
         <v>14</v>
@@ -1293,18 +1314,18 @@
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1328,18 +1349,18 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -1363,21 +1384,21 @@
         <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -1389,7 +1410,7 @@
         <v>256</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -1398,18 +1419,18 @@
         <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>10</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1433,18 +1454,18 @@
         <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1468,18 +1489,18 @@
         <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1494,7 +1515,7 @@
         <v>256</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1503,18 +1524,18 @@
         <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1546,10 +1567,10 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1573,21 +1594,21 @@
         <v>15</v>
       </c>
       <c r="J15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -1608,18 +1629,18 @@
         <v>15</v>
       </c>
       <c r="J16" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1643,18 +1664,18 @@
         <v>15</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K17" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1669,7 +1690,7 @@
         <v>256</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -1678,18 +1699,18 @@
         <v>15</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K18" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>18</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1713,18 +1734,18 @@
         <v>15</v>
       </c>
       <c r="J19" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1748,18 +1769,18 @@
         <v>15</v>
       </c>
       <c r="J20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K20" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1783,18 +1804,18 @@
         <v>15</v>
       </c>
       <c r="J21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22">
-        <v>21</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1818,21 +1839,21 @@
         <v>15</v>
       </c>
       <c r="J22" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K22" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1844,7 +1865,7 @@
         <v>256</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
@@ -1853,18 +1874,18 @@
         <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1888,27 +1909,27 @@
         <v>15</v>
       </c>
       <c r="J24" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K24" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E25">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F25">
         <v>256</v>
@@ -1923,19 +1944,19 @@
         <v>15</v>
       </c>
       <c r="J25" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
@@ -1958,24 +1979,24 @@
         <v>15</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K26" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -1993,18 +2014,18 @@
         <v>15</v>
       </c>
       <c r="J27" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K27" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -2028,21 +2049,21 @@
         <v>15</v>
       </c>
       <c r="J28" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K28" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
         <v>13</v>
@@ -2063,18 +2084,18 @@
         <v>15</v>
       </c>
       <c r="J29" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K29" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
@@ -2089,7 +2110,7 @@
         <v>256</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H30" t="s">
         <v>14</v>
@@ -2098,18 +2119,18 @@
         <v>15</v>
       </c>
       <c r="J30" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
@@ -2118,7 +2139,7 @@
         <v>13</v>
       </c>
       <c r="E31">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F31">
         <v>256</v>
@@ -2133,15 +2154,15 @@
         <v>15</v>
       </c>
       <c r="J31" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K31" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -2150,7 +2171,7 @@
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E32">
         <v>15</v>
@@ -2168,18 +2189,18 @@
         <v>15</v>
       </c>
       <c r="J32" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K32" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
@@ -2203,18 +2224,18 @@
         <v>15</v>
       </c>
       <c r="J33" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K33" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -2238,21 +2259,21 @@
         <v>15</v>
       </c>
       <c r="J34" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K34" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:11">
       <c r="A35">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -2264,7 +2285,7 @@
         <v>256</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H35" t="s">
         <v>14</v>
@@ -2281,7 +2302,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36">
-        <v>35</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
         <v>18</v>
@@ -2293,7 +2314,7 @@
         <v>13</v>
       </c>
       <c r="E36">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F36">
         <v>256</v>
@@ -2308,18 +2329,18 @@
         <v>15</v>
       </c>
       <c r="J36" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K36" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="A37">
-        <v>36</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
@@ -2343,24 +2364,24 @@
         <v>15</v>
       </c>
       <c r="J37" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K37" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:11">
       <c r="A38">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E38">
         <v>15</v>
@@ -2378,18 +2399,18 @@
         <v>15</v>
       </c>
       <c r="J38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K38" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="A39">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
@@ -2413,21 +2434,21 @@
         <v>15</v>
       </c>
       <c r="J39" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K39" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
         <v>13</v>
@@ -2448,18 +2469,18 @@
         <v>15</v>
       </c>
       <c r="J40" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K40" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:11">
       <c r="A41">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
@@ -2483,18 +2504,18 @@
         <v>15</v>
       </c>
       <c r="J41" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K41" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="A42">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
@@ -2503,13 +2524,13 @@
         <v>13</v>
       </c>
       <c r="E42">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F42">
         <v>256</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
@@ -2518,18 +2539,18 @@
         <v>15</v>
       </c>
       <c r="J42" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K42" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="43" spans="1:11">
       <c r="A43">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
@@ -2553,24 +2574,24 @@
         <v>15</v>
       </c>
       <c r="J43" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K43" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E44">
         <v>15</v>
@@ -2588,18 +2609,18 @@
         <v>15</v>
       </c>
       <c r="J44" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K44" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -2623,18 +2644,18 @@
         <v>15</v>
       </c>
       <c r="J45" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K45" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
         <v>12</v>
@@ -2658,15 +2679,15 @@
         <v>15</v>
       </c>
       <c r="J46" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K46" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
         <v>18</v>
@@ -2675,10 +2696,10 @@
         <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F47">
         <v>256</v>
@@ -2693,34 +2714,34 @@
         <v>15</v>
       </c>
       <c r="J47" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K47" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48">
+        <v>15</v>
+      </c>
+      <c r="F48">
+        <v>256</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48">
-        <v>15</v>
-      </c>
-      <c r="F48">
-        <v>256</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="H48" t="s">
         <v>14</v>
       </c>
@@ -2728,21 +2749,21 @@
         <v>15</v>
       </c>
       <c r="J48" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K48" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="A49">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
         <v>13</v>
@@ -2763,18 +2784,18 @@
         <v>15</v>
       </c>
       <c r="J49" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K49" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:11">
       <c r="A50">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
         <v>12</v>
@@ -2798,24 +2819,24 @@
         <v>15</v>
       </c>
       <c r="J50" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K50" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="A51">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C51" t="s">
         <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E51">
         <v>15</v>
@@ -2833,18 +2854,18 @@
         <v>15</v>
       </c>
       <c r="J51" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K51" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:11">
       <c r="A52">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C52" t="s">
         <v>12</v>
@@ -2853,7 +2874,7 @@
         <v>13</v>
       </c>
       <c r="E52">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F52">
         <v>256</v>
@@ -2868,18 +2889,18 @@
         <v>15</v>
       </c>
       <c r="J52" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K52" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="A53">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C53" t="s">
         <v>12</v>
@@ -2894,7 +2915,7 @@
         <v>256</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H53" t="s">
         <v>14</v>
@@ -2903,21 +2924,21 @@
         <v>15</v>
       </c>
       <c r="J53" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K53" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54">
-        <v>53</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
         <v>13</v>
@@ -2938,18 +2959,18 @@
         <v>15</v>
       </c>
       <c r="J54" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K54" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55">
-        <v>54</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C55" t="s">
         <v>12</v>
@@ -2973,18 +2994,18 @@
         <v>15</v>
       </c>
       <c r="J55" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K55" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C56" t="s">
         <v>12</v>
@@ -2993,7 +3014,7 @@
         <v>13</v>
       </c>
       <c r="E56">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F56">
         <v>256</v>
@@ -3008,18 +3029,18 @@
         <v>15</v>
       </c>
       <c r="J56" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K56" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="B57" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C57" t="s">
         <v>12</v>
@@ -3034,7 +3055,7 @@
         <v>256</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H57" t="s">
         <v>14</v>
@@ -3043,21 +3064,21 @@
         <v>15</v>
       </c>
       <c r="J57" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K57" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
         <v>18</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D58" t="s">
         <v>13</v>
@@ -3078,18 +3099,18 @@
         <v>15</v>
       </c>
       <c r="J58" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K58" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="A59">
-        <v>58</v>
+        <v>123</v>
       </c>
       <c r="B59" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C59" t="s">
         <v>12</v>
@@ -3113,18 +3134,18 @@
         <v>15</v>
       </c>
       <c r="J59" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K59" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:11">
       <c r="A60">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C60" t="s">
         <v>12</v>
@@ -3148,21 +3169,21 @@
         <v>15</v>
       </c>
       <c r="J60" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K60" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="A61">
-        <v>60</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D61" t="s">
         <v>13</v>
@@ -3183,18 +3204,18 @@
         <v>15</v>
       </c>
       <c r="J61" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K61" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:11">
       <c r="A62">
-        <v>61</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C62" t="s">
         <v>12</v>
@@ -3218,18 +3239,18 @@
         <v>15</v>
       </c>
       <c r="J62" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K62" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="A63">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B63" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C63" t="s">
         <v>12</v>
@@ -3253,24 +3274,24 @@
         <v>15</v>
       </c>
       <c r="J63" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K63" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E64">
         <v>15</v>
@@ -3288,18 +3309,18 @@
         <v>15</v>
       </c>
       <c r="J64" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K64" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65">
-        <v>64</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C65" t="s">
         <v>12</v>
@@ -3323,18 +3344,18 @@
         <v>15</v>
       </c>
       <c r="J65" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K65" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:11">
       <c r="A66">
-        <v>65</v>
+        <v>130</v>
       </c>
       <c r="B66" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -3358,24 +3379,24 @@
         <v>15</v>
       </c>
       <c r="J66" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K66" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:11">
       <c r="A67">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C67" t="s">
         <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="E67">
         <v>15</v>
@@ -3393,10 +3414,10 @@
         <v>15</v>
       </c>
       <c r="J67" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K67" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3424,33 +3445,27 @@
     <hyperlink ref="D22" r:id="rId1" display="128gb"/>
     <hyperlink ref="D23" r:id="rId1" display="128gb"/>
     <hyperlink ref="D24" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D25" r:id="rId1" display="128gb"/>
+    <hyperlink ref="D25" r:id="rId1" display="256gb"/>
     <hyperlink ref="D26" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D27" r:id="rId1" display="128gb"/>
     <hyperlink ref="D28" r:id="rId1" display="128gb"/>
     <hyperlink ref="D29" r:id="rId1" display="128gb"/>
     <hyperlink ref="D30" r:id="rId1" display="128gb"/>
     <hyperlink ref="D31" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D32" r:id="rId1" display="128gb"/>
     <hyperlink ref="D33" r:id="rId1" display="128gb"/>
     <hyperlink ref="D34" r:id="rId1" display="128gb"/>
     <hyperlink ref="D35" r:id="rId1" display="128gb"/>
     <hyperlink ref="D36" r:id="rId1" display="128gb"/>
     <hyperlink ref="D37" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D38" r:id="rId1" display="128gb"/>
     <hyperlink ref="D39" r:id="rId1" display="128gb"/>
     <hyperlink ref="D40" r:id="rId1" display="128gb"/>
     <hyperlink ref="D41" r:id="rId1" display="128gb"/>
     <hyperlink ref="D42" r:id="rId1" display="128gb"/>
     <hyperlink ref="D43" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D44" r:id="rId1" display="128gb"/>
     <hyperlink ref="D45" r:id="rId1" display="128gb"/>
     <hyperlink ref="D46" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D47" r:id="rId1" display="128gb"/>
     <hyperlink ref="D48" r:id="rId1" display="128gb"/>
     <hyperlink ref="D49" r:id="rId1" display="128gb"/>
     <hyperlink ref="D50" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D51" r:id="rId1" display="128gb"/>
     <hyperlink ref="D52" r:id="rId1" display="128gb"/>
     <hyperlink ref="D53" r:id="rId1" display="128gb"/>
     <hyperlink ref="D54" r:id="rId1" display="128gb"/>
@@ -3463,10 +3478,16 @@
     <hyperlink ref="D61" r:id="rId1" display="128gb"/>
     <hyperlink ref="D62" r:id="rId1" display="128gb"/>
     <hyperlink ref="D63" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D64" r:id="rId1" display="128gb"/>
     <hyperlink ref="D65" r:id="rId1" display="128gb"/>
     <hyperlink ref="D66" r:id="rId1" display="128gb"/>
-    <hyperlink ref="D67" r:id="rId1" display="128gb"/>
+    <hyperlink ref="D27" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D32" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D38" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D44" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D47" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D51" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D67" r:id="rId1" display="256gb"/>
+    <hyperlink ref="D64" r:id="rId1" display="256gb"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>